<commit_message>
Revisión de modulo SPOOLER remitente- destinatario
(EDISTRIBUTEUR, TB_EREMIT_DEST_TRAN_DOM_CP)
Generación archivo detalle de archivos y métodos que usan  las unidades.
Spooler Nueva versión (se revisó el resultado de los store)
Cambio de esquema de objetos de objetos  “SC_RS”
</commit_message>
<xml_diff>
--- a/00-Documentacion/remite/spooler/remiten spooler.xlsx
+++ b/00-Documentacion/remite/spooler/remiten spooler.xlsx
@@ -5,27 +5,36 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\Raul\remite\spooler\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\remite\spooler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD6E123-7796-438E-B737-B16A25C49A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD8D13FF-A727-4945-B6D8-6077B17E1B87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="361">
   <si>
     <t>unidad</t>
   </si>
@@ -694,6 +703,420 @@
   </si>
   <si>
     <t>Command</t>
+  </si>
+  <si>
+    <t>EDIRECCIONES_ENTREGA,EDISTRIBUTEUR</t>
+  </si>
+  <si>
+    <t>Anexo24.bas</t>
+  </si>
+  <si>
+    <t>EDISTRIBUTEUR</t>
+  </si>
+  <si>
+    <t>anex24</t>
+  </si>
+  <si>
+    <t>Backlog_mod2.bas</t>
+  </si>
+  <si>
+    <t>SQL2</t>
+  </si>
+  <si>
+    <t>backlog2</t>
+  </si>
+  <si>
+    <t>Backlog_mot_vin_mod.bas</t>
+  </si>
+  <si>
+    <t>backlog2_mot_vin</t>
+  </si>
+  <si>
+    <t>Bosch_pedimentos2_mod.bas</t>
+  </si>
+  <si>
+    <t>Bosch_Pedimentos2</t>
+  </si>
+  <si>
+    <t>Bosch_pedimentos3_mod.bas</t>
+  </si>
+  <si>
+    <t>SQL_03</t>
+  </si>
+  <si>
+    <t>Bosch_pedimentos3_mod_R</t>
+  </si>
+  <si>
+    <t>Bosch_Pedimentos3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bosch_pedimentos3_xls_mod.bas </t>
+  </si>
+  <si>
+    <t>Bosch_Pedimentos3_xls</t>
+  </si>
+  <si>
+    <t>Bosch_pedimentos_mod.bas</t>
+  </si>
+  <si>
+    <t>Bosch_Pedimentos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cove_generacion_xml_mod.bas </t>
+  </si>
+  <si>
+    <t>cove_generacion_xml</t>
+  </si>
+  <si>
+    <t>Datos_fact_pedto.bas</t>
+  </si>
+  <si>
+    <t>Datos_fct_pedto</t>
+  </si>
+  <si>
+    <t>Dicat_fiscal.bas</t>
+  </si>
+  <si>
+    <t>dict_fiscal</t>
+  </si>
+  <si>
+    <t>trading_embarques_zarpe.bas</t>
+  </si>
+  <si>
+    <t>embarques_zarpe</t>
+  </si>
+  <si>
+    <t>transmission.bas</t>
+  </si>
+  <si>
+    <t>trans_reporte</t>
+  </si>
+  <si>
+    <t>web_anexo24_aero_mod.bas</t>
+  </si>
+  <si>
+    <t>anexo_24_aero</t>
+  </si>
+  <si>
+    <t>web_anexo24_casadiaz_mod.bas</t>
+  </si>
+  <si>
+    <t>web_anexo24_Cooper.bas</t>
+  </si>
+  <si>
+    <t>anexo24_cooper</t>
+  </si>
+  <si>
+    <t>web_anexo24_gkn.bas</t>
+  </si>
+  <si>
+    <t>SQL_D</t>
+  </si>
+  <si>
+    <t>anexo24_IK_plastic</t>
+  </si>
+  <si>
+    <t>web_anexo24_GKN_det_mod.bas</t>
+  </si>
+  <si>
+    <t>anex24_GKN_det</t>
+  </si>
+  <si>
+    <t>web_anexo24_IK_plastic.bas</t>
+  </si>
+  <si>
+    <t>web_anexo24_int_point_mod.bas</t>
+  </si>
+  <si>
+    <t>anx24_int_point</t>
+  </si>
+  <si>
+    <t>web_anexo24_monsanto2.bas</t>
+  </si>
+  <si>
+    <t>anexo24_monsanto2</t>
+  </si>
+  <si>
+    <t>web_anexo24_monsanto_mod.bas</t>
+  </si>
+  <si>
+    <t>anexo24_monsanto</t>
+  </si>
+  <si>
+    <t>web_anexo24_scj_R1_mod.bas</t>
+  </si>
+  <si>
+    <t>anexo24_scj_R1</t>
+  </si>
+  <si>
+    <t>web_anexo24_volvo_mod.bas</t>
+  </si>
+  <si>
+    <t>anexo24_volvo</t>
+  </si>
+  <si>
+    <t>web_anixter_mod.bas</t>
+  </si>
+  <si>
+    <t>anixter_gastos</t>
+  </si>
+  <si>
+    <t>web_control_invent_eurocopter_mod.bas</t>
+  </si>
+  <si>
+    <t>control_invent_eurocopter</t>
+  </si>
+  <si>
+    <t>web_descarga_masiva_partes.bas</t>
+  </si>
+  <si>
+    <t>descarga_masiva_partes</t>
+  </si>
+  <si>
+    <t>web_facturas_conceptos_magnetti_fol.bas</t>
+  </si>
+  <si>
+    <t>web_facturas_conceptos_magnetti_fol</t>
+  </si>
+  <si>
+    <t>web_facturas_conceptos_magnetti_mod.bas</t>
+  </si>
+  <si>
+    <t>web_facturas_conceptos_magnetti</t>
+  </si>
+  <si>
+    <t>web_facturas_johnson.bas</t>
+  </si>
+  <si>
+    <t>facturas_johnson</t>
+  </si>
+  <si>
+    <t>web_facturas_mod.bas</t>
+  </si>
+  <si>
+    <t>facturas_txt</t>
+  </si>
+  <si>
+    <t>web_fmc_reporte_mod.bas</t>
+  </si>
+  <si>
+    <t>web_fmc_reporte</t>
+  </si>
+  <si>
+    <t>web_ftp_digit_Tupperware_mod.bas</t>
+  </si>
+  <si>
+    <t>SQL_PED</t>
+  </si>
+  <si>
+    <t>ftp_digit_tupperware</t>
+  </si>
+  <si>
+    <t>web_gkn_exportacion_mod.bas</t>
+  </si>
+  <si>
+    <t>SQL_Rep</t>
+  </si>
+  <si>
+    <t>gkn_exportacion</t>
+  </si>
+  <si>
+    <t>web_hbpo_anx24_mod.bas</t>
+  </si>
+  <si>
+    <t>hbpo_anx24</t>
+  </si>
+  <si>
+    <t>web_honda_anexo24_mod.bas</t>
+  </si>
+  <si>
+    <t>honda_anexo24</t>
+  </si>
+  <si>
+    <t>web_lista_refs_mod.bas</t>
+  </si>
+  <si>
+    <t>lista_refs</t>
+  </si>
+  <si>
+    <t>web_logis_catalogos.bas</t>
+  </si>
+  <si>
+    <t>logis_catalogos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">web_logis_invoices.bas </t>
+  </si>
+  <si>
+    <t>logis_invoices</t>
+  </si>
+  <si>
+    <t>web_logis_invoices_bosch.bas</t>
+  </si>
+  <si>
+    <t>logis_invoices_bosch</t>
+  </si>
+  <si>
+    <t>web_logis_invoices_faurecia_mod.bas</t>
+  </si>
+  <si>
+    <t>logis_invoices_faurecia</t>
+  </si>
+  <si>
+    <t>web_logis_invoices_firmenich.bas</t>
+  </si>
+  <si>
+    <t>logis_invoices_firmenich</t>
+  </si>
+  <si>
+    <t>web_logis_invoices_loreal.bas</t>
+  </si>
+  <si>
+    <t>logis_invoices_loreal</t>
+  </si>
+  <si>
+    <t>web_logis_invoice_firmenich2_mod.bas</t>
+  </si>
+  <si>
+    <t>logis_invoices_firmenich2</t>
+  </si>
+  <si>
+    <t>web_monsanto_relacion_fac_mod.bas</t>
+  </si>
+  <si>
+    <t>monsanto_relacion_fac</t>
+  </si>
+  <si>
+    <t>web_operaciones_volvo.bas</t>
+  </si>
+  <si>
+    <t>operacion_volvo</t>
+  </si>
+  <si>
+    <t>web_pedimentos_absormex_mod.bas</t>
+  </si>
+  <si>
+    <t>SQL_PEDTO_Absormex_DETALLE</t>
+  </si>
+  <si>
+    <t>pedimentos_absormex</t>
+  </si>
+  <si>
+    <t>web_pedimentos_cotemar_mod.bas</t>
+  </si>
+  <si>
+    <t>pedimentos_cotemar</t>
+  </si>
+  <si>
+    <t>web_pedimento_pdf_instant.bas</t>
+  </si>
+  <si>
+    <t>pedimento_pdf_instant</t>
+  </si>
+  <si>
+    <t>web_pedimento_pdf_instant_130922.bas</t>
+  </si>
+  <si>
+    <t>web_pedim_pdf_antolin_his_mod.bas</t>
+  </si>
+  <si>
+    <t>SQL_PEDTO</t>
+  </si>
+  <si>
+    <t>pedim_pdf_antolin_his,generacion_pedim_edocs</t>
+  </si>
+  <si>
+    <t>web_pedim_pdf_antolin_mod.bas</t>
+  </si>
+  <si>
+    <t>pedim_pdf_antolin</t>
+  </si>
+  <si>
+    <t>web_pedim_pdf_magneti_mod.bas</t>
+  </si>
+  <si>
+    <t>pedim_pdf_magneti</t>
+  </si>
+  <si>
+    <t>web_pedim_SCI_2_mod.bas</t>
+  </si>
+  <si>
+    <t>web_pedimentos_SCI_2</t>
+  </si>
+  <si>
+    <t>web_pedim_SCI_mod.bas</t>
+  </si>
+  <si>
+    <t>web_pedimentos_SCI</t>
+  </si>
+  <si>
+    <t>web_ped_vs_invoice.bas</t>
+  </si>
+  <si>
+    <t>ped_invoices</t>
+  </si>
+  <si>
+    <t>web_ped_vs_invoices_apasco_mod.bas</t>
+  </si>
+  <si>
+    <t>ped_invoices_apasco</t>
+  </si>
+  <si>
+    <t>web_PO_mod.bas</t>
+  </si>
+  <si>
+    <t>web_reporte_PO</t>
+  </si>
+  <si>
+    <t>web_remesas_mod.bas</t>
+  </si>
+  <si>
+    <t>web_remesas</t>
+  </si>
+  <si>
+    <t>web_reservacion_CD_mod.bas</t>
+  </si>
+  <si>
+    <t>reservacion_CD</t>
+  </si>
+  <si>
+    <t>web_reservacion_LTL_excel.bas</t>
+  </si>
+  <si>
+    <t>reservacion_ltl_excel</t>
+  </si>
+  <si>
+    <t>web_reservacion_LTL_mod.bas</t>
+  </si>
+  <si>
+    <t>reservacion_ltl</t>
+  </si>
+  <si>
+    <t>web_scj_pendiente_despacho.bas</t>
+  </si>
+  <si>
+    <t>SQL_PEND_DESP</t>
+  </si>
+  <si>
+    <t>scj_pendiente_despacho</t>
+  </si>
+  <si>
+    <t>web_supp_invoice.bas</t>
+  </si>
+  <si>
+    <t>supp_invoice</t>
+  </si>
+  <si>
+    <t>web_supp_invoices_fonkel.bas</t>
+  </si>
+  <si>
+    <t>supp_invoice_fonkel</t>
+  </si>
+  <si>
+    <t>web_talones_pdf_mod.bas</t>
+  </si>
+  <si>
+    <t>talones_pdf</t>
   </si>
 </sst>
 </file>
@@ -1042,18 +1465,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E132"/>
+  <dimension ref="A1:E203"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="B169" sqref="B169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1078,7 +1502,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>223</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
@@ -1287,7 +1711,7 @@
         <v>31</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>5</v>
+        <v>223</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>32</v>
@@ -1384,7 +1808,7 @@
         <v>43</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>5</v>
+        <v>223</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>6</v>
@@ -1554,7 +1978,7 @@
         <v>63</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>5</v>
+        <v>223</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>6</v>
@@ -1614,7 +2038,7 @@
         <v>73</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>5</v>
+        <v>223</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>69</v>
@@ -1629,7 +2053,7 @@
         <v>75</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>5</v>
+        <v>223</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>69</v>
@@ -1704,7 +2128,7 @@
         <v>87</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>5</v>
+        <v>223</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>32</v>
@@ -2332,7 +2756,7 @@
         <v>144</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>5</v>
+        <v>223</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>6</v>
@@ -2373,7 +2797,7 @@
         <v>149</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>5</v>
+        <v>223</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>6</v>
@@ -2418,7 +2842,7 @@
         <v>154</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>5</v>
+        <v>223</v>
       </c>
       <c r="C98" s="2" t="s">
         <v>6</v>
@@ -2463,7 +2887,7 @@
         <v>160</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>5</v>
+        <v>223</v>
       </c>
       <c r="C101" s="2" t="s">
         <v>6</v>
@@ -2508,7 +2932,7 @@
         <v>166</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>5</v>
+        <v>223</v>
       </c>
       <c r="C104" s="2" t="s">
         <v>167</v>
@@ -2596,7 +3020,7 @@
         <v>177</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>5</v>
+        <v>223</v>
       </c>
       <c r="C110" s="2" t="s">
         <v>6</v>
@@ -2772,7 +3196,7 @@
         <v>200</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>5</v>
+        <v>223</v>
       </c>
       <c r="C122" s="2" t="s">
         <v>96</v>
@@ -2830,7 +3254,7 @@
         <v>207</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>5</v>
+        <v>223</v>
       </c>
       <c r="C126" s="2" t="s">
         <v>6</v>
@@ -2845,7 +3269,7 @@
         <v>209</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>5</v>
+        <v>223</v>
       </c>
       <c r="C127" s="2" t="s">
         <v>6</v>
@@ -2920,7 +3344,7 @@
         <v>220</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>5</v>
+        <v>223</v>
       </c>
       <c r="C132" s="2" t="s">
         <v>6</v>
@@ -2929,6 +3353,1061 @@
         <v>221</v>
       </c>
       <c r="E132" s="2"/>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D133" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E133" s="2"/>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="E134" s="2"/>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D135" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="E135" s="2"/>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D136" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="E136" s="2"/>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D137" s="2"/>
+      <c r="E137" s="2"/>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D138" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="E138" s="2"/>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D139" s="2"/>
+      <c r="E139" s="2"/>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D140" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="E140" s="2"/>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D141" s="2"/>
+      <c r="E141" s="2"/>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D142" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="E142" s="2"/>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D143" s="2"/>
+      <c r="E143" s="2"/>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D144" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="E144" s="2"/>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D145" s="2"/>
+      <c r="E145" s="2"/>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="E146" s="2"/>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D147" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="E147" s="2"/>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D148" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="E148" s="2"/>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D149" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="E149" s="2"/>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D150" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="E150" s="2"/>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D151" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E151" s="2"/>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D152" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E152" s="2"/>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D153" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="E153" s="2"/>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="D154" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="E154" s="2"/>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D155" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="E155" s="2"/>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="D156" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="E156" s="2"/>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D157" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="E157" s="2"/>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A158" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C158" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D158" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="E158" s="2"/>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A159" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D159" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="E159" s="2"/>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D160" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="E160" s="2"/>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D161" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="E161" s="2"/>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D162" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="E162" s="2"/>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D163" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="E163" s="2"/>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D164" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="E164" s="2"/>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C165" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D165" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="E165" s="2"/>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D166" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="E166" s="2"/>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D167" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="E167" s="2"/>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A168" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C168" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D168" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="E168" s="2"/>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C169" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D169" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="E169" s="2"/>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C170" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D170" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="E170" s="2"/>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C171" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D171" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="E171" s="2"/>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C172" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D172" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="E172" s="2"/>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C173" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D173" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="E173" s="2"/>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C174" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D174" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="E174" s="2"/>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C175" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D175" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="E175" s="2"/>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C176" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D176" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="E176" s="2"/>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A177" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C177" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D177" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="E177" s="2"/>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A178" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C178" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D178" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="E178" s="2"/>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A179" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C179" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D179" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="E179" s="2"/>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A180" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D180" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="E180" s="2"/>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A181" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D181" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="E181" s="2"/>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A182" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C182" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D182" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="E182" s="2"/>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A183" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C183" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D183" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="E183" s="2"/>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A184" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="D184" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="E184" s="2"/>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A185" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C185" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D185" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="E185" s="2"/>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A186" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="B186" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C186" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D186" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="E186" s="2"/>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A187" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C187" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D187" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="E187" s="2"/>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A188" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="B188" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C188" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="D188" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E188" s="2"/>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A189" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="B189" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C189" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="D189" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="E189" s="2"/>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A190" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B190" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C190" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="D190" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="E190" s="2"/>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A191" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C191" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D191" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="E191" s="2"/>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A192" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C192" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D192" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="E192" s="2"/>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A193" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B193" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C193" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D193" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="E193" s="2"/>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B194" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C194" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D194" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="E194" s="2"/>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A195" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C195" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D195" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="E195" s="2"/>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A196" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="B196" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C196" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D196" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="E196" s="2"/>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A197" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C197" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D197" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="E197" s="2"/>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A198" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B198" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C198" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D198" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="E198" s="2"/>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A199" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B199" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C199" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D199" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="E199" s="2"/>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A200" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B200" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C200" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="D200" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="E200" s="2"/>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B201" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C201" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D201" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="E201" s="2"/>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B202" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C202" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D202" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="E202" s="2"/>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="B203" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C203" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D203" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="E203" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>